<commit_message>
Se agrego el requerimiento 7
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\ProyectoMetodologia\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\proyectometodologia7342\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAFDDF7-E3DC-4B57-A19F-EEDC657D1EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66FCFBC5-0291-4609-A468-4F8468BC42F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>Requisito</t>
   </si>
@@ -89,12 +88,15 @@
   </si>
   <si>
     <t>RQ5: El sistema debe permitir ingresar la cantidad de billetes y monedas en caja al final de cada día laborable, así como realizar el cálculo del arqueo de caja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RQ7: Si el usuario desea dar de baja a un empleado existente, comunicará al sistema el nombre de usuario del empleado y si  existe, el usuario podrá darlo de baja. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,14 +522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24A3371-B552-49DB-8C90-07F078E5FB0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
@@ -648,7 +653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
@@ -729,6 +734,33 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="16" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>11</v>
@@ -736,5 +768,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregado documentacion de especificacion de requisitos de software, y modificado los requisitos 8 y 10
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\proyectometodologia7342\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\ProyectoMetodologia\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB47596-12A3-4BC7-AEBF-BA667C7D3E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,13 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -93,19 +87,19 @@
     <t xml:space="preserve">RQ7: Si el usuario desea dar de baja a un empleado existente, comunicará al sistema el nombre de usuario del empleado y si  existe, el usuario podrá darlo de baja. </t>
   </si>
   <si>
-    <t>RQ8: Si el operario desea editar su información personal, el sistema debe permitirlo.</t>
-  </si>
-  <si>
-    <t>RQ9: Si el cliente desea cambiar algun dato personal registrado en el sistema, el sistema debe emitir una confirmación por pantalla al operario, y seguidamente enviar un correo al cliente con los nuevos datos que se encuentran en el sistema.</t>
-  </si>
-  <si>
-    <t>RQ10: El sistema debe llevar la cuenta de ventas que se van haciendo durante el dia en cada uno de los cajeros que esten en operación.</t>
+    <t>RQ8: Si el operario desea editar su información personal, el sistema debe permitirlo, a excepción de su C.I/C.C</t>
+  </si>
+  <si>
+    <t>RQ9: Si el cliente desea cambiar algun dato personal registrado en el sistema, el sistema debe comunicar al operario el cual realizará el cambio de la información en el sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RQ10: El sistema debe realizar el cálculo de arqueo de caja en base a la información ingresada por el usuario de la cantidad de billetes y monedas recibidas. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,14 +525,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
@@ -662,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
@@ -770,7 +764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
@@ -797,7 +791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
@@ -824,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Agregado documentacion de especificacion de requisitos de software en pdf y docx, y modificado los requisitos 8 y 10
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\proyectometodologia7342\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\ProyectoMetodologia\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB47596-12A3-4BC7-AEBF-BA667C7D3E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,13 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -93,19 +87,19 @@
     <t xml:space="preserve">RQ7: Si el usuario desea dar de baja a un empleado existente, comunicará al sistema el nombre de usuario del empleado y si  existe, el usuario podrá darlo de baja. </t>
   </si>
   <si>
-    <t>RQ8: Si el operario desea editar su información personal, el sistema debe permitirlo.</t>
-  </si>
-  <si>
-    <t>RQ9: Si el cliente desea cambiar algun dato personal registrado en el sistema, el sistema debe emitir una confirmación por pantalla al operario, y seguidamente enviar un correo al cliente con los nuevos datos que se encuentran en el sistema.</t>
-  </si>
-  <si>
-    <t>RQ10: El sistema debe llevar la cuenta de ventas que se van haciendo durante el dia en cada uno de los cajeros que esten en operación.</t>
+    <t>RQ8: Si el operario desea editar su información personal, el sistema debe permitirlo, a excepción de su C.I/C.C</t>
+  </si>
+  <si>
+    <t>RQ9: Si el cliente desea cambiar algun dato personal registrado en el sistema, el sistema debe comunicar al operario el cual realizará el cambio de la información en el sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RQ10: El sistema debe realizar el cálculo de arqueo de caja en base a la información ingresada por el usuario de la cantidad de billetes y monedas recibidas. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,14 +525,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
@@ -662,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
@@ -770,7 +764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
@@ -797,7 +791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
@@ -824,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>

</xml_diff>